<commit_message>
- BC hoahong hanghoa - chi tiet:  add column {GiaTriSauHeSo}
</commit_message>
<xml_diff>
--- a/banhang24/Template/ExportExcel/Report/BaoCaoChietKhau/Temp_BaoCaoHoaHongHangHoa_ChiTiet.xlsx
+++ b/banhang24/Template/ExportExcel/Report/BaoCaoChietKhau/Temp_BaoCaoHoaHongHangHoa_ChiTiet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
   <si>
     <t>BÁO CÁO CHI TIẾT HOA HỒNG THEO NHÂN VIÊN</t>
   </si>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t>Hệ số</t>
+  </si>
+  <si>
+    <t>Giá trị sau hệ số</t>
   </si>
 </sst>
 </file>
@@ -345,6 +348,48 @@
     <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -357,12 +402,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="3" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -374,42 +413,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -692,7 +695,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X30"/>
+  <dimension ref="A1:Y30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
@@ -708,47 +711,49 @@
     <col min="11" max="11" width="21.85546875" style="5" customWidth="1"/>
     <col min="12" max="12" width="34.28515625" style="5" customWidth="1"/>
     <col min="13" max="13" width="19.85546875" style="29" customWidth="1"/>
-    <col min="14" max="14" width="28.140625" style="6" customWidth="1"/>
-    <col min="15" max="15" width="12.5703125" style="52" customWidth="1"/>
-    <col min="16" max="16" width="15.42578125" style="45" customWidth="1"/>
-    <col min="17" max="19" width="16.7109375" style="6" customWidth="1"/>
-    <col min="20" max="20" width="15.42578125" style="13" customWidth="1"/>
-    <col min="21" max="21" width="16.7109375" style="6" customWidth="1"/>
-    <col min="22" max="22" width="17" style="6" customWidth="1"/>
-    <col min="23" max="23" width="20.140625" style="6" customWidth="1"/>
-    <col min="24" max="24" width="17.28515625" style="18" customWidth="1"/>
-    <col min="25" max="16384" width="9.140625" style="2"/>
+    <col min="14" max="14" width="25.5703125" style="6" customWidth="1"/>
+    <col min="15" max="15" width="14.7109375" style="6" customWidth="1"/>
+    <col min="16" max="16" width="21.7109375" style="36" customWidth="1"/>
+    <col min="17" max="17" width="15.42578125" style="31" customWidth="1"/>
+    <col min="18" max="20" width="16.7109375" style="6" customWidth="1"/>
+    <col min="21" max="21" width="15.42578125" style="13" customWidth="1"/>
+    <col min="22" max="22" width="16.7109375" style="6" customWidth="1"/>
+    <col min="23" max="23" width="17" style="6" customWidth="1"/>
+    <col min="24" max="24" width="20.140625" style="6" customWidth="1"/>
+    <col min="25" max="25" width="17.28515625" style="18" customWidth="1"/>
+    <col min="26" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:25" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31"/>
-      <c r="O1" s="31"/>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="31"/>
-      <c r="R1" s="31"/>
-      <c r="S1" s="31"/>
-      <c r="T1" s="31"/>
-      <c r="U1" s="31"/>
-      <c r="V1" s="1"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
+      <c r="N1" s="45"/>
+      <c r="O1" s="45"/>
+      <c r="P1" s="45"/>
+      <c r="Q1" s="45"/>
+      <c r="R1" s="45"/>
+      <c r="S1" s="45"/>
+      <c r="T1" s="45"/>
+      <c r="U1" s="45"/>
+      <c r="V1" s="45"/>
       <c r="W1" s="1"/>
-      <c r="X1" s="17"/>
-    </row>
-    <row r="2" spans="1:24" s="25" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X1" s="1"/>
+      <c r="Y1" s="17"/>
+    </row>
+    <row r="2" spans="1:25" s="25" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="23"/>
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
@@ -763,18 +768,19 @@
       <c r="L2" s="23"/>
       <c r="M2" s="28"/>
       <c r="N2" s="30"/>
-      <c r="O2" s="46"/>
-      <c r="P2" s="24"/>
-      <c r="Q2" s="23"/>
+      <c r="O2" s="30"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="24"/>
       <c r="R2" s="23"/>
       <c r="S2" s="23"/>
       <c r="T2" s="23"/>
       <c r="U2" s="23"/>
       <c r="V2" s="23"/>
       <c r="W2" s="23"/>
-      <c r="X2" s="24"/>
-    </row>
-    <row r="3" spans="1:24" s="25" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X2" s="23"/>
+      <c r="Y2" s="24"/>
+    </row>
+    <row r="3" spans="1:25" s="25" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="23"/>
       <c r="B3" s="23"/>
       <c r="C3" s="23"/>
@@ -789,126 +795,131 @@
       <c r="L3" s="23"/>
       <c r="M3" s="23"/>
       <c r="N3" s="23"/>
-      <c r="O3" s="47"/>
-      <c r="P3" s="24"/>
-      <c r="Q3" s="23"/>
+      <c r="O3" s="23"/>
+      <c r="P3" s="33"/>
+      <c r="Q3" s="24"/>
       <c r="R3" s="23"/>
       <c r="S3" s="23"/>
       <c r="T3" s="23"/>
       <c r="U3" s="23"/>
       <c r="V3" s="23"/>
       <c r="W3" s="23"/>
-      <c r="X3" s="26"/>
-    </row>
-    <row r="4" spans="1:24" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="35" t="s">
+      <c r="X3" s="23"/>
+      <c r="Y3" s="26"/>
+    </row>
+    <row r="4" spans="1:25" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="39" t="s">
+      <c r="C4" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="39" t="s">
+      <c r="D4" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="39" t="s">
+      <c r="E4" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="39" t="s">
+      <c r="F4" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="35" t="s">
+      <c r="G4" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="35" t="s">
+      <c r="H4" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="35" t="s">
+      <c r="I4" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="35" t="s">
+      <c r="J4" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="K4" s="35" t="s">
+      <c r="K4" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="L4" s="35" t="s">
+      <c r="L4" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="M4" s="35" t="s">
+      <c r="M4" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="N4" s="43" t="s">
+      <c r="N4" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="O4" s="48" t="s">
+      <c r="O4" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="P4" s="41" t="s">
+      <c r="P4" s="43" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q4" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="42"/>
-      <c r="R4" s="41" t="s">
+      <c r="R4" s="42"/>
+      <c r="S4" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="S4" s="42"/>
-      <c r="T4" s="41" t="s">
+      <c r="T4" s="42"/>
+      <c r="U4" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="U4" s="42"/>
-      <c r="V4" s="41" t="s">
+      <c r="V4" s="42"/>
+      <c r="W4" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="W4" s="42"/>
-      <c r="X4" s="43" t="s">
+      <c r="X4" s="42"/>
+      <c r="Y4" s="37" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:24" s="7" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="36"/>
-      <c r="B5" s="38"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="36"/>
-      <c r="I5" s="36"/>
-      <c r="J5" s="36"/>
-      <c r="K5" s="36"/>
-      <c r="L5" s="36"/>
-      <c r="M5" s="36"/>
-      <c r="N5" s="44"/>
-      <c r="O5" s="49"/>
-      <c r="P5" s="19" t="s">
+    <row r="5" spans="1:25" s="7" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="40"/>
+      <c r="B5" s="50"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="40"/>
+      <c r="J5" s="40"/>
+      <c r="K5" s="40"/>
+      <c r="L5" s="40"/>
+      <c r="M5" s="40"/>
+      <c r="N5" s="38"/>
+      <c r="O5" s="38"/>
+      <c r="P5" s="44"/>
+      <c r="Q5" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="Q5" s="19" t="s">
+      <c r="R5" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="R5" s="19" t="s">
+      <c r="S5" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="S5" s="19" t="s">
+      <c r="T5" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="T5" s="19" t="s">
+      <c r="U5" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="U5" s="19" t="s">
+      <c r="V5" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="V5" s="19" t="s">
+      <c r="W5" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="W5" s="19" t="s">
+      <c r="X5" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="X5" s="44"/>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y5" s="38"/>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6" s="9"/>
       <c r="C6" s="22"/>
@@ -923,18 +934,19 @@
       <c r="L6" s="8"/>
       <c r="M6" s="14"/>
       <c r="N6" s="10"/>
-      <c r="O6" s="50"/>
-      <c r="P6" s="10"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="34"/>
       <c r="Q6" s="10"/>
       <c r="R6" s="10"/>
       <c r="S6" s="10"/>
-      <c r="T6" s="14"/>
-      <c r="U6" s="10"/>
+      <c r="T6" s="10"/>
+      <c r="U6" s="14"/>
       <c r="V6" s="10"/>
       <c r="W6" s="10"/>
-      <c r="X6" s="20"/>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X6" s="10"/>
+      <c r="Y6" s="20"/>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" s="9"/>
       <c r="C7" s="22"/>
@@ -949,18 +961,19 @@
       <c r="L7" s="8"/>
       <c r="M7" s="14"/>
       <c r="N7" s="10"/>
-      <c r="O7" s="50"/>
-      <c r="P7" s="10"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="34"/>
       <c r="Q7" s="10"/>
       <c r="R7" s="10"/>
       <c r="S7" s="10"/>
-      <c r="T7" s="14"/>
-      <c r="U7" s="10"/>
+      <c r="T7" s="10"/>
+      <c r="U7" s="14"/>
       <c r="V7" s="10"/>
       <c r="W7" s="10"/>
-      <c r="X7" s="20"/>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X7" s="10"/>
+      <c r="Y7" s="20"/>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="9"/>
       <c r="C8" s="22"/>
@@ -975,18 +988,19 @@
       <c r="L8" s="8"/>
       <c r="M8" s="14"/>
       <c r="N8" s="10"/>
-      <c r="O8" s="50"/>
-      <c r="P8" s="10"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="34"/>
       <c r="Q8" s="10"/>
       <c r="R8" s="10"/>
       <c r="S8" s="10"/>
-      <c r="T8" s="14"/>
-      <c r="U8" s="10"/>
+      <c r="T8" s="10"/>
+      <c r="U8" s="14"/>
       <c r="V8" s="10"/>
       <c r="W8" s="10"/>
-      <c r="X8" s="20"/>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X8" s="10"/>
+      <c r="Y8" s="20"/>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
       <c r="B9" s="9"/>
       <c r="C9" s="22"/>
@@ -1001,18 +1015,19 @@
       <c r="L9" s="8"/>
       <c r="M9" s="14"/>
       <c r="N9" s="10"/>
-      <c r="O9" s="50"/>
-      <c r="P9" s="10"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="34"/>
       <c r="Q9" s="10"/>
       <c r="R9" s="10"/>
       <c r="S9" s="10"/>
-      <c r="T9" s="14"/>
-      <c r="U9" s="10"/>
+      <c r="T9" s="10"/>
+      <c r="U9" s="14"/>
       <c r="V9" s="10"/>
       <c r="W9" s="10"/>
-      <c r="X9" s="20"/>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X9" s="10"/>
+      <c r="Y9" s="20"/>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
       <c r="B10" s="9"/>
       <c r="C10" s="22"/>
@@ -1027,18 +1042,19 @@
       <c r="L10" s="8"/>
       <c r="M10" s="14"/>
       <c r="N10" s="10"/>
-      <c r="O10" s="50"/>
-      <c r="P10" s="10"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="34"/>
       <c r="Q10" s="10"/>
       <c r="R10" s="10"/>
       <c r="S10" s="10"/>
-      <c r="T10" s="14"/>
-      <c r="U10" s="10"/>
+      <c r="T10" s="10"/>
+      <c r="U10" s="14"/>
       <c r="V10" s="10"/>
       <c r="W10" s="10"/>
-      <c r="X10" s="20"/>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X10" s="10"/>
+      <c r="Y10" s="20"/>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="B11" s="9"/>
       <c r="C11" s="22"/>
@@ -1053,18 +1069,19 @@
       <c r="L11" s="8"/>
       <c r="M11" s="14"/>
       <c r="N11" s="10"/>
-      <c r="O11" s="50"/>
-      <c r="P11" s="10"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="34"/>
       <c r="Q11" s="10"/>
       <c r="R11" s="10"/>
       <c r="S11" s="10"/>
-      <c r="T11" s="14"/>
-      <c r="U11" s="10"/>
+      <c r="T11" s="10"/>
+      <c r="U11" s="14"/>
       <c r="V11" s="10"/>
       <c r="W11" s="10"/>
-      <c r="X11" s="20"/>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X11" s="10"/>
+      <c r="Y11" s="20"/>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
       <c r="B12" s="9"/>
       <c r="C12" s="22"/>
@@ -1079,18 +1096,19 @@
       <c r="L12" s="8"/>
       <c r="M12" s="14"/>
       <c r="N12" s="10"/>
-      <c r="O12" s="50"/>
-      <c r="P12" s="10"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="34"/>
       <c r="Q12" s="10"/>
       <c r="R12" s="10"/>
       <c r="S12" s="10"/>
-      <c r="T12" s="14"/>
-      <c r="U12" s="10"/>
+      <c r="T12" s="10"/>
+      <c r="U12" s="14"/>
       <c r="V12" s="10"/>
       <c r="W12" s="10"/>
-      <c r="X12" s="20"/>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X12" s="10"/>
+      <c r="Y12" s="20"/>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
       <c r="B13" s="9"/>
       <c r="C13" s="22"/>
@@ -1105,18 +1123,19 @@
       <c r="L13" s="8"/>
       <c r="M13" s="14"/>
       <c r="N13" s="10"/>
-      <c r="O13" s="50"/>
-      <c r="P13" s="10"/>
+      <c r="O13" s="10"/>
+      <c r="P13" s="34"/>
       <c r="Q13" s="10"/>
       <c r="R13" s="10"/>
       <c r="S13" s="10"/>
-      <c r="T13" s="14"/>
-      <c r="U13" s="10"/>
+      <c r="T13" s="10"/>
+      <c r="U13" s="14"/>
       <c r="V13" s="10"/>
       <c r="W13" s="10"/>
-      <c r="X13" s="20"/>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X13" s="10"/>
+      <c r="Y13" s="20"/>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
       <c r="B14" s="9"/>
       <c r="C14" s="22"/>
@@ -1131,18 +1150,19 @@
       <c r="L14" s="8"/>
       <c r="M14" s="14"/>
       <c r="N14" s="10"/>
-      <c r="O14" s="50"/>
-      <c r="P14" s="10"/>
+      <c r="O14" s="10"/>
+      <c r="P14" s="34"/>
       <c r="Q14" s="10"/>
       <c r="R14" s="10"/>
       <c r="S14" s="10"/>
-      <c r="T14" s="14"/>
-      <c r="U14" s="10"/>
+      <c r="T14" s="10"/>
+      <c r="U14" s="14"/>
       <c r="V14" s="10"/>
       <c r="W14" s="10"/>
-      <c r="X14" s="20"/>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X14" s="10"/>
+      <c r="Y14" s="20"/>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
       <c r="B15" s="9"/>
       <c r="C15" s="22"/>
@@ -1157,18 +1177,19 @@
       <c r="L15" s="8"/>
       <c r="M15" s="14"/>
       <c r="N15" s="10"/>
-      <c r="O15" s="50"/>
-      <c r="P15" s="10"/>
+      <c r="O15" s="10"/>
+      <c r="P15" s="34"/>
       <c r="Q15" s="10"/>
       <c r="R15" s="10"/>
       <c r="S15" s="10"/>
-      <c r="T15" s="14"/>
-      <c r="U15" s="10"/>
+      <c r="T15" s="10"/>
+      <c r="U15" s="14"/>
       <c r="V15" s="10"/>
       <c r="W15" s="10"/>
-      <c r="X15" s="20"/>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X15" s="10"/>
+      <c r="Y15" s="20"/>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
       <c r="B16" s="9"/>
       <c r="C16" s="22"/>
@@ -1183,18 +1204,19 @@
       <c r="L16" s="8"/>
       <c r="M16" s="14"/>
       <c r="N16" s="10"/>
-      <c r="O16" s="50"/>
-      <c r="P16" s="10"/>
+      <c r="O16" s="10"/>
+      <c r="P16" s="34"/>
       <c r="Q16" s="10"/>
       <c r="R16" s="10"/>
       <c r="S16" s="10"/>
-      <c r="T16" s="14"/>
-      <c r="U16" s="10"/>
+      <c r="T16" s="10"/>
+      <c r="U16" s="14"/>
       <c r="V16" s="10"/>
       <c r="W16" s="10"/>
-      <c r="X16" s="20"/>
-    </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X16" s="10"/>
+      <c r="Y16" s="20"/>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
       <c r="B17" s="9"/>
       <c r="C17" s="22"/>
@@ -1209,18 +1231,19 @@
       <c r="L17" s="8"/>
       <c r="M17" s="14"/>
       <c r="N17" s="10"/>
-      <c r="O17" s="50"/>
-      <c r="P17" s="10"/>
+      <c r="O17" s="10"/>
+      <c r="P17" s="34"/>
       <c r="Q17" s="10"/>
       <c r="R17" s="10"/>
       <c r="S17" s="10"/>
-      <c r="T17" s="14"/>
-      <c r="U17" s="10"/>
+      <c r="T17" s="10"/>
+      <c r="U17" s="14"/>
       <c r="V17" s="10"/>
       <c r="W17" s="10"/>
-      <c r="X17" s="20"/>
-    </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X17" s="10"/>
+      <c r="Y17" s="20"/>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
       <c r="B18" s="9"/>
       <c r="C18" s="22"/>
@@ -1235,18 +1258,19 @@
       <c r="L18" s="8"/>
       <c r="M18" s="14"/>
       <c r="N18" s="10"/>
-      <c r="O18" s="50"/>
-      <c r="P18" s="10"/>
+      <c r="O18" s="10"/>
+      <c r="P18" s="34"/>
       <c r="Q18" s="10"/>
       <c r="R18" s="10"/>
       <c r="S18" s="10"/>
-      <c r="T18" s="14"/>
-      <c r="U18" s="10"/>
+      <c r="T18" s="10"/>
+      <c r="U18" s="14"/>
       <c r="V18" s="10"/>
       <c r="W18" s="10"/>
-      <c r="X18" s="20"/>
-    </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X18" s="10"/>
+      <c r="Y18" s="20"/>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19" s="9"/>
       <c r="C19" s="22"/>
@@ -1261,18 +1285,19 @@
       <c r="L19" s="8"/>
       <c r="M19" s="14"/>
       <c r="N19" s="10"/>
-      <c r="O19" s="50"/>
-      <c r="P19" s="10"/>
+      <c r="O19" s="10"/>
+      <c r="P19" s="34"/>
       <c r="Q19" s="10"/>
       <c r="R19" s="10"/>
       <c r="S19" s="10"/>
-      <c r="T19" s="14"/>
-      <c r="U19" s="10"/>
+      <c r="T19" s="10"/>
+      <c r="U19" s="14"/>
       <c r="V19" s="10"/>
       <c r="W19" s="10"/>
-      <c r="X19" s="20"/>
-    </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X19" s="10"/>
+      <c r="Y19" s="20"/>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
       <c r="B20" s="9"/>
       <c r="C20" s="22"/>
@@ -1287,18 +1312,19 @@
       <c r="L20" s="8"/>
       <c r="M20" s="14"/>
       <c r="N20" s="10"/>
-      <c r="O20" s="50"/>
-      <c r="P20" s="10"/>
+      <c r="O20" s="10"/>
+      <c r="P20" s="34"/>
       <c r="Q20" s="10"/>
       <c r="R20" s="10"/>
       <c r="S20" s="10"/>
-      <c r="T20" s="14"/>
-      <c r="U20" s="10"/>
+      <c r="T20" s="10"/>
+      <c r="U20" s="14"/>
       <c r="V20" s="10"/>
       <c r="W20" s="10"/>
-      <c r="X20" s="20"/>
-    </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X20" s="10"/>
+      <c r="Y20" s="20"/>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
       <c r="B21" s="9"/>
       <c r="C21" s="22"/>
@@ -1313,18 +1339,19 @@
       <c r="L21" s="8"/>
       <c r="M21" s="14"/>
       <c r="N21" s="10"/>
-      <c r="O21" s="50"/>
-      <c r="P21" s="10"/>
+      <c r="O21" s="10"/>
+      <c r="P21" s="34"/>
       <c r="Q21" s="10"/>
       <c r="R21" s="10"/>
       <c r="S21" s="10"/>
-      <c r="T21" s="14"/>
-      <c r="U21" s="10"/>
+      <c r="T21" s="10"/>
+      <c r="U21" s="14"/>
       <c r="V21" s="10"/>
       <c r="W21" s="10"/>
-      <c r="X21" s="20"/>
-    </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X21" s="10"/>
+      <c r="Y21" s="20"/>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
       <c r="B22" s="9"/>
       <c r="C22" s="22"/>
@@ -1339,18 +1366,19 @@
       <c r="L22" s="8"/>
       <c r="M22" s="14"/>
       <c r="N22" s="10"/>
-      <c r="O22" s="50"/>
-      <c r="P22" s="10"/>
+      <c r="O22" s="10"/>
+      <c r="P22" s="34"/>
       <c r="Q22" s="10"/>
       <c r="R22" s="10"/>
       <c r="S22" s="10"/>
-      <c r="T22" s="14"/>
-      <c r="U22" s="10"/>
+      <c r="T22" s="10"/>
+      <c r="U22" s="14"/>
       <c r="V22" s="10"/>
       <c r="W22" s="10"/>
-      <c r="X22" s="20"/>
-    </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X22" s="10"/>
+      <c r="Y22" s="20"/>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
       <c r="B23" s="9"/>
       <c r="C23" s="22"/>
@@ -1365,18 +1393,19 @@
       <c r="L23" s="8"/>
       <c r="M23" s="14"/>
       <c r="N23" s="10"/>
-      <c r="O23" s="50"/>
-      <c r="P23" s="10"/>
+      <c r="O23" s="10"/>
+      <c r="P23" s="34"/>
       <c r="Q23" s="10"/>
       <c r="R23" s="10"/>
       <c r="S23" s="10"/>
-      <c r="T23" s="14"/>
-      <c r="U23" s="10"/>
+      <c r="T23" s="10"/>
+      <c r="U23" s="14"/>
       <c r="V23" s="10"/>
       <c r="W23" s="10"/>
-      <c r="X23" s="20"/>
-    </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X23" s="10"/>
+      <c r="Y23" s="20"/>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
       <c r="B24" s="9"/>
       <c r="C24" s="22"/>
@@ -1391,18 +1420,19 @@
       <c r="L24" s="8"/>
       <c r="M24" s="14"/>
       <c r="N24" s="10"/>
-      <c r="O24" s="50"/>
-      <c r="P24" s="10"/>
+      <c r="O24" s="10"/>
+      <c r="P24" s="34"/>
       <c r="Q24" s="10"/>
       <c r="R24" s="10"/>
       <c r="S24" s="10"/>
-      <c r="T24" s="14"/>
-      <c r="U24" s="10"/>
+      <c r="T24" s="10"/>
+      <c r="U24" s="14"/>
       <c r="V24" s="10"/>
       <c r="W24" s="10"/>
-      <c r="X24" s="20"/>
-    </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X24" s="10"/>
+      <c r="Y24" s="20"/>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" s="8"/>
       <c r="B25" s="9"/>
       <c r="C25" s="22"/>
@@ -1417,18 +1447,19 @@
       <c r="L25" s="8"/>
       <c r="M25" s="14"/>
       <c r="N25" s="10"/>
-      <c r="O25" s="50"/>
-      <c r="P25" s="10"/>
+      <c r="O25" s="10"/>
+      <c r="P25" s="34"/>
       <c r="Q25" s="10"/>
       <c r="R25" s="10"/>
       <c r="S25" s="10"/>
-      <c r="T25" s="14"/>
-      <c r="U25" s="10"/>
+      <c r="T25" s="10"/>
+      <c r="U25" s="14"/>
       <c r="V25" s="10"/>
       <c r="W25" s="10"/>
-      <c r="X25" s="20"/>
-    </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X25" s="10"/>
+      <c r="Y25" s="20"/>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
       <c r="B26" s="9"/>
       <c r="C26" s="22"/>
@@ -1443,18 +1474,19 @@
       <c r="L26" s="8"/>
       <c r="M26" s="14"/>
       <c r="N26" s="10"/>
-      <c r="O26" s="50"/>
-      <c r="P26" s="10"/>
+      <c r="O26" s="10"/>
+      <c r="P26" s="34"/>
       <c r="Q26" s="10"/>
       <c r="R26" s="10"/>
       <c r="S26" s="10"/>
-      <c r="T26" s="14"/>
-      <c r="U26" s="10"/>
+      <c r="T26" s="10"/>
+      <c r="U26" s="14"/>
       <c r="V26" s="10"/>
       <c r="W26" s="10"/>
-      <c r="X26" s="20"/>
-    </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X26" s="10"/>
+      <c r="Y26" s="20"/>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A27" s="8"/>
       <c r="B27" s="9"/>
       <c r="C27" s="22"/>
@@ -1469,18 +1501,19 @@
       <c r="L27" s="8"/>
       <c r="M27" s="14"/>
       <c r="N27" s="10"/>
-      <c r="O27" s="50"/>
-      <c r="P27" s="10"/>
+      <c r="O27" s="10"/>
+      <c r="P27" s="34"/>
       <c r="Q27" s="10"/>
       <c r="R27" s="10"/>
       <c r="S27" s="10"/>
-      <c r="T27" s="14"/>
-      <c r="U27" s="10"/>
+      <c r="T27" s="10"/>
+      <c r="U27" s="14"/>
       <c r="V27" s="10"/>
       <c r="W27" s="10"/>
-      <c r="X27" s="20"/>
-    </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X27" s="10"/>
+      <c r="Y27" s="20"/>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A28" s="8"/>
       <c r="B28" s="9"/>
       <c r="C28" s="22"/>
@@ -1495,18 +1528,19 @@
       <c r="L28" s="8"/>
       <c r="M28" s="14"/>
       <c r="N28" s="10"/>
-      <c r="O28" s="50"/>
-      <c r="P28" s="10"/>
+      <c r="O28" s="10"/>
+      <c r="P28" s="34"/>
       <c r="Q28" s="10"/>
       <c r="R28" s="10"/>
       <c r="S28" s="10"/>
-      <c r="T28" s="14"/>
-      <c r="U28" s="10"/>
+      <c r="T28" s="10"/>
+      <c r="U28" s="14"/>
       <c r="V28" s="10"/>
       <c r="W28" s="10"/>
-      <c r="X28" s="20"/>
-    </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X28" s="10"/>
+      <c r="Y28" s="20"/>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A29" s="8"/>
       <c r="B29" s="9"/>
       <c r="C29" s="22"/>
@@ -1521,32 +1555,33 @@
       <c r="L29" s="8"/>
       <c r="M29" s="14"/>
       <c r="N29" s="10"/>
-      <c r="O29" s="50"/>
-      <c r="P29" s="10"/>
+      <c r="O29" s="10"/>
+      <c r="P29" s="34"/>
       <c r="Q29" s="10"/>
       <c r="R29" s="10"/>
       <c r="S29" s="10"/>
-      <c r="T29" s="14"/>
-      <c r="U29" s="10"/>
+      <c r="T29" s="10"/>
+      <c r="U29" s="14"/>
       <c r="V29" s="10"/>
       <c r="W29" s="10"/>
-      <c r="X29" s="20"/>
-    </row>
-    <row r="30" spans="1:24" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="32" t="s">
+      <c r="X29" s="10"/>
+      <c r="Y29" s="20"/>
+    </row>
+    <row r="30" spans="1:25" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="33"/>
-      <c r="I30" s="33"/>
-      <c r="J30" s="33"/>
-      <c r="K30" s="33"/>
-      <c r="L30" s="34"/>
+      <c r="B30" s="47"/>
+      <c r="C30" s="47"/>
+      <c r="D30" s="47"/>
+      <c r="E30" s="47"/>
+      <c r="F30" s="47"/>
+      <c r="G30" s="47"/>
+      <c r="H30" s="47"/>
+      <c r="I30" s="47"/>
+      <c r="J30" s="47"/>
+      <c r="K30" s="47"/>
+      <c r="L30" s="48"/>
       <c r="M30" s="15">
         <f>SUM(M$6:M29)</f>
         <v>0</v>
@@ -1555,41 +1590,36 @@
         <f>SUM(N$6:N29)</f>
         <v>0</v>
       </c>
-      <c r="O30" s="51"/>
-      <c r="P30" s="16"/>
-      <c r="Q30" s="11">
-        <f>SUM(Q$6:Q29)</f>
+      <c r="O30" s="16"/>
+      <c r="P30" s="35"/>
+      <c r="Q30" s="16"/>
+      <c r="R30" s="11">
+        <f>SUM(R$6:R29)</f>
         <v>0</v>
       </c>
-      <c r="R30" s="27"/>
-      <c r="S30" s="27">
-        <f xml:space="preserve"> SUM(S$6:S29)</f>
+      <c r="S30" s="27"/>
+      <c r="T30" s="27">
+        <f xml:space="preserve"> SUM(T$6:T29)</f>
         <v>0</v>
       </c>
-      <c r="T30" s="15"/>
-      <c r="U30" s="11">
-        <f>SUM(U$6:U29)</f>
+      <c r="U30" s="15"/>
+      <c r="V30" s="11">
+        <f>SUM(V$6:V29)</f>
         <v>0</v>
       </c>
-      <c r="V30" s="11"/>
-      <c r="W30" s="11">
-        <f>SUM(W$6:W29)</f>
+      <c r="W30" s="11"/>
+      <c r="X30" s="11">
+        <f>SUM(X$6:X29)</f>
         <v>0</v>
       </c>
-      <c r="X30" s="11">
-        <f>SUM($X$6:X29)</f>
+      <c r="Y30" s="11">
+        <f>SUM($Y$6:Y29)</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="X4:X5"/>
-    <mergeCell ref="L4:L5"/>
-    <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="T4:U4"/>
-    <mergeCell ref="V4:W4"/>
-    <mergeCell ref="O4:O5"/>
-    <mergeCell ref="A1:U1"/>
+  <mergeCells count="23">
+    <mergeCell ref="A1:V1"/>
     <mergeCell ref="A30:L30"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="B4:B5"/>
@@ -1601,10 +1631,17 @@
     <mergeCell ref="I4:I5"/>
     <mergeCell ref="J4:J5"/>
     <mergeCell ref="K4:K5"/>
-    <mergeCell ref="R4:S4"/>
+    <mergeCell ref="S4:T4"/>
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="M4:M5"/>
     <mergeCell ref="N4:N5"/>
+    <mergeCell ref="Y4:Y5"/>
+    <mergeCell ref="L4:L5"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="W4:X4"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="O4:O5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>

</xml_diff>

<commit_message>
- BC hoahong - hanghoa chitiet: add column {NVPhuTrach}
</commit_message>
<xml_diff>
--- a/banhang24/Template/ExportExcel/Report/BaoCaoChietKhau/Temp_BaoCaoHoaHongHangHoa_ChiTiet.xlsx
+++ b/banhang24/Template/ExportExcel/Report/BaoCaoChietKhau/Temp_BaoCaoHoaHongHangHoa_ChiTiet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
   <si>
     <t>BÁO CÁO CHI TIẾT HOA HỒNG THEO NHÂN VIÊN</t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t>Giá trị sau hệ số</t>
+  </si>
+  <si>
+    <t>NV phụ trách</t>
   </si>
 </sst>
 </file>
@@ -366,52 +369,52 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="3" fontId="3" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="3" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="3" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -695,65 +698,66 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y30"/>
+  <dimension ref="A1:Z30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.28515625" style="5" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" style="3" customWidth="1"/>
-    <col min="3" max="6" width="19.42578125" style="21" customWidth="1"/>
-    <col min="7" max="10" width="19.85546875" style="4" customWidth="1"/>
-    <col min="11" max="11" width="21.85546875" style="5" customWidth="1"/>
-    <col min="12" max="12" width="34.28515625" style="5" customWidth="1"/>
-    <col min="13" max="13" width="19.85546875" style="29" customWidth="1"/>
-    <col min="14" max="14" width="25.5703125" style="6" customWidth="1"/>
-    <col min="15" max="15" width="14.7109375" style="6" customWidth="1"/>
-    <col min="16" max="16" width="21.7109375" style="36" customWidth="1"/>
-    <col min="17" max="17" width="15.42578125" style="31" customWidth="1"/>
-    <col min="18" max="20" width="16.7109375" style="6" customWidth="1"/>
-    <col min="21" max="21" width="15.42578125" style="13" customWidth="1"/>
-    <col min="22" max="22" width="16.7109375" style="6" customWidth="1"/>
-    <col min="23" max="23" width="17" style="6" customWidth="1"/>
-    <col min="24" max="24" width="20.140625" style="6" customWidth="1"/>
-    <col min="25" max="25" width="17.28515625" style="18" customWidth="1"/>
-    <col min="26" max="16384" width="9.140625" style="2"/>
+    <col min="3" max="7" width="19.42578125" style="21" customWidth="1"/>
+    <col min="8" max="11" width="19.85546875" style="4" customWidth="1"/>
+    <col min="12" max="12" width="21.85546875" style="5" customWidth="1"/>
+    <col min="13" max="13" width="34.28515625" style="5" customWidth="1"/>
+    <col min="14" max="14" width="19.85546875" style="29" customWidth="1"/>
+    <col min="15" max="15" width="25.5703125" style="6" customWidth="1"/>
+    <col min="16" max="16" width="14.7109375" style="6" customWidth="1"/>
+    <col min="17" max="17" width="21.7109375" style="36" customWidth="1"/>
+    <col min="18" max="18" width="15.42578125" style="31" customWidth="1"/>
+    <col min="19" max="21" width="16.7109375" style="6" customWidth="1"/>
+    <col min="22" max="22" width="15.42578125" style="13" customWidth="1"/>
+    <col min="23" max="23" width="16.7109375" style="6" customWidth="1"/>
+    <col min="24" max="24" width="17" style="6" customWidth="1"/>
+    <col min="25" max="25" width="20.140625" style="6" customWidth="1"/>
+    <col min="26" max="26" width="17.28515625" style="18" customWidth="1"/>
+    <col min="27" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+    <row r="1" spans="1:26" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
-      <c r="Q1" s="45"/>
-      <c r="R1" s="45"/>
-      <c r="S1" s="45"/>
-      <c r="T1" s="45"/>
-      <c r="U1" s="45"/>
-      <c r="V1" s="45"/>
-      <c r="W1" s="1"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="37"/>
+      <c r="P1" s="37"/>
+      <c r="Q1" s="37"/>
+      <c r="R1" s="37"/>
+      <c r="S1" s="37"/>
+      <c r="T1" s="37"/>
+      <c r="U1" s="37"/>
+      <c r="V1" s="37"/>
+      <c r="W1" s="37"/>
       <c r="X1" s="1"/>
-      <c r="Y1" s="17"/>
-    </row>
-    <row r="2" spans="1:25" s="25" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="17"/>
+    </row>
+    <row r="2" spans="1:26" s="25" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="23"/>
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
@@ -766,21 +770,22 @@
       <c r="J2" s="23"/>
       <c r="K2" s="23"/>
       <c r="L2" s="23"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="30"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="28"/>
       <c r="O2" s="30"/>
-      <c r="P2" s="32"/>
-      <c r="Q2" s="24"/>
-      <c r="R2" s="23"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="24"/>
       <c r="S2" s="23"/>
       <c r="T2" s="23"/>
       <c r="U2" s="23"/>
       <c r="V2" s="23"/>
       <c r="W2" s="23"/>
       <c r="X2" s="23"/>
-      <c r="Y2" s="24"/>
-    </row>
-    <row r="3" spans="1:25" s="25" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Y2" s="23"/>
+      <c r="Z2" s="24"/>
+    </row>
+    <row r="3" spans="1:26" s="25" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="23"/>
       <c r="B3" s="23"/>
       <c r="C3" s="23"/>
@@ -796,851 +801,882 @@
       <c r="M3" s="23"/>
       <c r="N3" s="23"/>
       <c r="O3" s="23"/>
-      <c r="P3" s="33"/>
-      <c r="Q3" s="24"/>
-      <c r="R3" s="23"/>
+      <c r="P3" s="23"/>
+      <c r="Q3" s="33"/>
+      <c r="R3" s="24"/>
       <c r="S3" s="23"/>
       <c r="T3" s="23"/>
       <c r="U3" s="23"/>
       <c r="V3" s="23"/>
       <c r="W3" s="23"/>
       <c r="X3" s="23"/>
-      <c r="Y3" s="26"/>
-    </row>
-    <row r="4" spans="1:25" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="39" t="s">
+      <c r="Y3" s="23"/>
+      <c r="Z3" s="26"/>
+    </row>
+    <row r="4" spans="1:26" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="49" t="s">
+      <c r="B4" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="51" t="s">
+      <c r="C4" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="51" t="s">
+      <c r="D4" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="51" t="s">
+      <c r="E4" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="51" t="s">
+      <c r="F4" s="45" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="39" t="s">
+      <c r="H4" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="39" t="s">
+      <c r="I4" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="39" t="s">
+      <c r="J4" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="39" t="s">
+      <c r="K4" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="K4" s="39" t="s">
+      <c r="L4" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="L4" s="39" t="s">
+      <c r="M4" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="M4" s="39" t="s">
+      <c r="N4" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="N4" s="37" t="s">
+      <c r="O4" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="O4" s="37" t="s">
+      <c r="P4" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="P4" s="43" t="s">
+      <c r="Q4" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="Q4" s="41" t="s">
+      <c r="R4" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="R4" s="42"/>
-      <c r="S4" s="41" t="s">
+      <c r="S4" s="48"/>
+      <c r="T4" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="T4" s="42"/>
-      <c r="U4" s="41" t="s">
+      <c r="U4" s="48"/>
+      <c r="V4" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="V4" s="42"/>
-      <c r="W4" s="41" t="s">
+      <c r="W4" s="48"/>
+      <c r="X4" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="X4" s="42"/>
-      <c r="Y4" s="37" t="s">
+      <c r="Y4" s="48"/>
+      <c r="Z4" s="49" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:25" s="7" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="40"/>
-      <c r="B5" s="50"/>
-      <c r="C5" s="52"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
-      <c r="F5" s="52"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="40"/>
-      <c r="I5" s="40"/>
-      <c r="J5" s="40"/>
-      <c r="K5" s="40"/>
-      <c r="L5" s="40"/>
-      <c r="M5" s="40"/>
-      <c r="N5" s="38"/>
-      <c r="O5" s="38"/>
-      <c r="P5" s="44"/>
-      <c r="Q5" s="19" t="s">
+    <row r="5" spans="1:26" s="7" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="42"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="42"/>
+      <c r="I5" s="42"/>
+      <c r="J5" s="42"/>
+      <c r="K5" s="42"/>
+      <c r="L5" s="42"/>
+      <c r="M5" s="42"/>
+      <c r="N5" s="42"/>
+      <c r="O5" s="50"/>
+      <c r="P5" s="50"/>
+      <c r="Q5" s="52"/>
+      <c r="R5" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="R5" s="19" t="s">
+      <c r="S5" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="S5" s="19" t="s">
+      <c r="T5" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="T5" s="19" t="s">
+      <c r="U5" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="U5" s="19" t="s">
+      <c r="V5" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="V5" s="19" t="s">
+      <c r="W5" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="W5" s="19" t="s">
+      <c r="X5" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="X5" s="19" t="s">
+      <c r="Y5" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="Y5" s="38"/>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z5" s="50"/>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6" s="9"/>
       <c r="C6" s="22"/>
       <c r="D6" s="22"/>
       <c r="E6" s="22"/>
       <c r="F6" s="22"/>
-      <c r="G6" s="8"/>
+      <c r="G6" s="22"/>
       <c r="H6" s="8"/>
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
       <c r="L6" s="8"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="10"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="14"/>
       <c r="O6" s="10"/>
-      <c r="P6" s="34"/>
-      <c r="Q6" s="10"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="34"/>
       <c r="R6" s="10"/>
       <c r="S6" s="10"/>
       <c r="T6" s="10"/>
-      <c r="U6" s="14"/>
-      <c r="V6" s="10"/>
+      <c r="U6" s="10"/>
+      <c r="V6" s="14"/>
       <c r="W6" s="10"/>
       <c r="X6" s="10"/>
-      <c r="Y6" s="20"/>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y6" s="10"/>
+      <c r="Z6" s="20"/>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" s="9"/>
       <c r="C7" s="22"/>
       <c r="D7" s="22"/>
       <c r="E7" s="22"/>
       <c r="F7" s="22"/>
-      <c r="G7" s="8"/>
+      <c r="G7" s="22"/>
       <c r="H7" s="8"/>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
       <c r="K7" s="8"/>
       <c r="L7" s="8"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="10"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="14"/>
       <c r="O7" s="10"/>
-      <c r="P7" s="34"/>
-      <c r="Q7" s="10"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="34"/>
       <c r="R7" s="10"/>
       <c r="S7" s="10"/>
       <c r="T7" s="10"/>
-      <c r="U7" s="14"/>
-      <c r="V7" s="10"/>
+      <c r="U7" s="10"/>
+      <c r="V7" s="14"/>
       <c r="W7" s="10"/>
       <c r="X7" s="10"/>
-      <c r="Y7" s="20"/>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y7" s="10"/>
+      <c r="Z7" s="20"/>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="9"/>
       <c r="C8" s="22"/>
       <c r="D8" s="22"/>
       <c r="E8" s="22"/>
       <c r="F8" s="22"/>
-      <c r="G8" s="8"/>
+      <c r="G8" s="22"/>
       <c r="H8" s="8"/>
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>
       <c r="L8" s="8"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="10"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="14"/>
       <c r="O8" s="10"/>
-      <c r="P8" s="34"/>
-      <c r="Q8" s="10"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="34"/>
       <c r="R8" s="10"/>
       <c r="S8" s="10"/>
       <c r="T8" s="10"/>
-      <c r="U8" s="14"/>
-      <c r="V8" s="10"/>
+      <c r="U8" s="10"/>
+      <c r="V8" s="14"/>
       <c r="W8" s="10"/>
       <c r="X8" s="10"/>
-      <c r="Y8" s="20"/>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y8" s="10"/>
+      <c r="Z8" s="20"/>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
       <c r="B9" s="9"/>
       <c r="C9" s="22"/>
       <c r="D9" s="22"/>
       <c r="E9" s="22"/>
       <c r="F9" s="22"/>
-      <c r="G9" s="8"/>
+      <c r="G9" s="22"/>
       <c r="H9" s="8"/>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
       <c r="L9" s="8"/>
-      <c r="M9" s="14"/>
-      <c r="N9" s="10"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="14"/>
       <c r="O9" s="10"/>
-      <c r="P9" s="34"/>
-      <c r="Q9" s="10"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="34"/>
       <c r="R9" s="10"/>
       <c r="S9" s="10"/>
       <c r="T9" s="10"/>
-      <c r="U9" s="14"/>
-      <c r="V9" s="10"/>
+      <c r="U9" s="10"/>
+      <c r="V9" s="14"/>
       <c r="W9" s="10"/>
       <c r="X9" s="10"/>
-      <c r="Y9" s="20"/>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y9" s="10"/>
+      <c r="Z9" s="20"/>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
       <c r="B10" s="9"/>
       <c r="C10" s="22"/>
       <c r="D10" s="22"/>
       <c r="E10" s="22"/>
       <c r="F10" s="22"/>
-      <c r="G10" s="8"/>
+      <c r="G10" s="22"/>
       <c r="H10" s="8"/>
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
       <c r="L10" s="8"/>
-      <c r="M10" s="14"/>
-      <c r="N10" s="10"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="14"/>
       <c r="O10" s="10"/>
-      <c r="P10" s="34"/>
-      <c r="Q10" s="10"/>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="34"/>
       <c r="R10" s="10"/>
       <c r="S10" s="10"/>
       <c r="T10" s="10"/>
-      <c r="U10" s="14"/>
-      <c r="V10" s="10"/>
+      <c r="U10" s="10"/>
+      <c r="V10" s="14"/>
       <c r="W10" s="10"/>
       <c r="X10" s="10"/>
-      <c r="Y10" s="20"/>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y10" s="10"/>
+      <c r="Z10" s="20"/>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="B11" s="9"/>
       <c r="C11" s="22"/>
       <c r="D11" s="22"/>
       <c r="E11" s="22"/>
       <c r="F11" s="22"/>
-      <c r="G11" s="8"/>
+      <c r="G11" s="22"/>
       <c r="H11" s="8"/>
       <c r="I11" s="8"/>
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
       <c r="L11" s="8"/>
-      <c r="M11" s="14"/>
-      <c r="N11" s="10"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="14"/>
       <c r="O11" s="10"/>
-      <c r="P11" s="34"/>
-      <c r="Q11" s="10"/>
+      <c r="P11" s="10"/>
+      <c r="Q11" s="34"/>
       <c r="R11" s="10"/>
       <c r="S11" s="10"/>
       <c r="T11" s="10"/>
-      <c r="U11" s="14"/>
-      <c r="V11" s="10"/>
+      <c r="U11" s="10"/>
+      <c r="V11" s="14"/>
       <c r="W11" s="10"/>
       <c r="X11" s="10"/>
-      <c r="Y11" s="20"/>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y11" s="10"/>
+      <c r="Z11" s="20"/>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
       <c r="B12" s="9"/>
       <c r="C12" s="22"/>
       <c r="D12" s="22"/>
       <c r="E12" s="22"/>
       <c r="F12" s="22"/>
-      <c r="G12" s="8"/>
+      <c r="G12" s="22"/>
       <c r="H12" s="8"/>
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
       <c r="L12" s="8"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="10"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="14"/>
       <c r="O12" s="10"/>
-      <c r="P12" s="34"/>
-      <c r="Q12" s="10"/>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="34"/>
       <c r="R12" s="10"/>
       <c r="S12" s="10"/>
       <c r="T12" s="10"/>
-      <c r="U12" s="14"/>
-      <c r="V12" s="10"/>
+      <c r="U12" s="10"/>
+      <c r="V12" s="14"/>
       <c r="W12" s="10"/>
       <c r="X12" s="10"/>
-      <c r="Y12" s="20"/>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y12" s="10"/>
+      <c r="Z12" s="20"/>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
       <c r="B13" s="9"/>
       <c r="C13" s="22"/>
       <c r="D13" s="22"/>
       <c r="E13" s="22"/>
       <c r="F13" s="22"/>
-      <c r="G13" s="8"/>
+      <c r="G13" s="22"/>
       <c r="H13" s="8"/>
       <c r="I13" s="8"/>
       <c r="J13" s="8"/>
       <c r="K13" s="8"/>
       <c r="L13" s="8"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="10"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="14"/>
       <c r="O13" s="10"/>
-      <c r="P13" s="34"/>
-      <c r="Q13" s="10"/>
+      <c r="P13" s="10"/>
+      <c r="Q13" s="34"/>
       <c r="R13" s="10"/>
       <c r="S13" s="10"/>
       <c r="T13" s="10"/>
-      <c r="U13" s="14"/>
-      <c r="V13" s="10"/>
+      <c r="U13" s="10"/>
+      <c r="V13" s="14"/>
       <c r="W13" s="10"/>
       <c r="X13" s="10"/>
-      <c r="Y13" s="20"/>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y13" s="10"/>
+      <c r="Z13" s="20"/>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
       <c r="B14" s="9"/>
       <c r="C14" s="22"/>
       <c r="D14" s="22"/>
       <c r="E14" s="22"/>
       <c r="F14" s="22"/>
-      <c r="G14" s="8"/>
+      <c r="G14" s="22"/>
       <c r="H14" s="8"/>
       <c r="I14" s="8"/>
       <c r="J14" s="8"/>
       <c r="K14" s="8"/>
       <c r="L14" s="8"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="10"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="14"/>
       <c r="O14" s="10"/>
-      <c r="P14" s="34"/>
-      <c r="Q14" s="10"/>
+      <c r="P14" s="10"/>
+      <c r="Q14" s="34"/>
       <c r="R14" s="10"/>
       <c r="S14" s="10"/>
       <c r="T14" s="10"/>
-      <c r="U14" s="14"/>
-      <c r="V14" s="10"/>
+      <c r="U14" s="10"/>
+      <c r="V14" s="14"/>
       <c r="W14" s="10"/>
       <c r="X14" s="10"/>
-      <c r="Y14" s="20"/>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y14" s="10"/>
+      <c r="Z14" s="20"/>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
       <c r="B15" s="9"/>
       <c r="C15" s="22"/>
       <c r="D15" s="22"/>
       <c r="E15" s="22"/>
       <c r="F15" s="22"/>
-      <c r="G15" s="8"/>
+      <c r="G15" s="22"/>
       <c r="H15" s="8"/>
       <c r="I15" s="8"/>
       <c r="J15" s="8"/>
       <c r="K15" s="8"/>
       <c r="L15" s="8"/>
-      <c r="M15" s="14"/>
-      <c r="N15" s="10"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="14"/>
       <c r="O15" s="10"/>
-      <c r="P15" s="34"/>
-      <c r="Q15" s="10"/>
+      <c r="P15" s="10"/>
+      <c r="Q15" s="34"/>
       <c r="R15" s="10"/>
       <c r="S15" s="10"/>
       <c r="T15" s="10"/>
-      <c r="U15" s="14"/>
-      <c r="V15" s="10"/>
+      <c r="U15" s="10"/>
+      <c r="V15" s="14"/>
       <c r="W15" s="10"/>
       <c r="X15" s="10"/>
-      <c r="Y15" s="20"/>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y15" s="10"/>
+      <c r="Z15" s="20"/>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
       <c r="B16" s="9"/>
       <c r="C16" s="22"/>
       <c r="D16" s="22"/>
       <c r="E16" s="22"/>
       <c r="F16" s="22"/>
-      <c r="G16" s="8"/>
+      <c r="G16" s="22"/>
       <c r="H16" s="8"/>
       <c r="I16" s="8"/>
       <c r="J16" s="8"/>
       <c r="K16" s="8"/>
       <c r="L16" s="8"/>
-      <c r="M16" s="14"/>
-      <c r="N16" s="10"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="14"/>
       <c r="O16" s="10"/>
-      <c r="P16" s="34"/>
-      <c r="Q16" s="10"/>
+      <c r="P16" s="10"/>
+      <c r="Q16" s="34"/>
       <c r="R16" s="10"/>
       <c r="S16" s="10"/>
       <c r="T16" s="10"/>
-      <c r="U16" s="14"/>
-      <c r="V16" s="10"/>
+      <c r="U16" s="10"/>
+      <c r="V16" s="14"/>
       <c r="W16" s="10"/>
       <c r="X16" s="10"/>
-      <c r="Y16" s="20"/>
-    </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y16" s="10"/>
+      <c r="Z16" s="20"/>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
       <c r="B17" s="9"/>
       <c r="C17" s="22"/>
       <c r="D17" s="22"/>
       <c r="E17" s="22"/>
       <c r="F17" s="22"/>
-      <c r="G17" s="8"/>
+      <c r="G17" s="22"/>
       <c r="H17" s="8"/>
       <c r="I17" s="8"/>
       <c r="J17" s="8"/>
       <c r="K17" s="8"/>
       <c r="L17" s="8"/>
-      <c r="M17" s="14"/>
-      <c r="N17" s="10"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="14"/>
       <c r="O17" s="10"/>
-      <c r="P17" s="34"/>
-      <c r="Q17" s="10"/>
+      <c r="P17" s="10"/>
+      <c r="Q17" s="34"/>
       <c r="R17" s="10"/>
       <c r="S17" s="10"/>
       <c r="T17" s="10"/>
-      <c r="U17" s="14"/>
-      <c r="V17" s="10"/>
+      <c r="U17" s="10"/>
+      <c r="V17" s="14"/>
       <c r="W17" s="10"/>
       <c r="X17" s="10"/>
-      <c r="Y17" s="20"/>
-    </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y17" s="10"/>
+      <c r="Z17" s="20"/>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
       <c r="B18" s="9"/>
       <c r="C18" s="22"/>
       <c r="D18" s="22"/>
       <c r="E18" s="22"/>
       <c r="F18" s="22"/>
-      <c r="G18" s="8"/>
+      <c r="G18" s="22"/>
       <c r="H18" s="8"/>
       <c r="I18" s="8"/>
       <c r="J18" s="8"/>
       <c r="K18" s="8"/>
       <c r="L18" s="8"/>
-      <c r="M18" s="14"/>
-      <c r="N18" s="10"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="14"/>
       <c r="O18" s="10"/>
-      <c r="P18" s="34"/>
-      <c r="Q18" s="10"/>
+      <c r="P18" s="10"/>
+      <c r="Q18" s="34"/>
       <c r="R18" s="10"/>
       <c r="S18" s="10"/>
       <c r="T18" s="10"/>
-      <c r="U18" s="14"/>
-      <c r="V18" s="10"/>
+      <c r="U18" s="10"/>
+      <c r="V18" s="14"/>
       <c r="W18" s="10"/>
       <c r="X18" s="10"/>
-      <c r="Y18" s="20"/>
-    </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y18" s="10"/>
+      <c r="Z18" s="20"/>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19" s="9"/>
       <c r="C19" s="22"/>
       <c r="D19" s="22"/>
       <c r="E19" s="22"/>
       <c r="F19" s="22"/>
-      <c r="G19" s="8"/>
+      <c r="G19" s="22"/>
       <c r="H19" s="8"/>
       <c r="I19" s="8"/>
       <c r="J19" s="8"/>
       <c r="K19" s="8"/>
       <c r="L19" s="8"/>
-      <c r="M19" s="14"/>
-      <c r="N19" s="10"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="14"/>
       <c r="O19" s="10"/>
-      <c r="P19" s="34"/>
-      <c r="Q19" s="10"/>
+      <c r="P19" s="10"/>
+      <c r="Q19" s="34"/>
       <c r="R19" s="10"/>
       <c r="S19" s="10"/>
       <c r="T19" s="10"/>
-      <c r="U19" s="14"/>
-      <c r="V19" s="10"/>
+      <c r="U19" s="10"/>
+      <c r="V19" s="14"/>
       <c r="W19" s="10"/>
       <c r="X19" s="10"/>
-      <c r="Y19" s="20"/>
-    </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y19" s="10"/>
+      <c r="Z19" s="20"/>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
       <c r="B20" s="9"/>
       <c r="C20" s="22"/>
       <c r="D20" s="22"/>
       <c r="E20" s="22"/>
       <c r="F20" s="22"/>
-      <c r="G20" s="8"/>
+      <c r="G20" s="22"/>
       <c r="H20" s="8"/>
       <c r="I20" s="8"/>
       <c r="J20" s="8"/>
       <c r="K20" s="8"/>
       <c r="L20" s="8"/>
-      <c r="M20" s="14"/>
-      <c r="N20" s="10"/>
+      <c r="M20" s="8"/>
+      <c r="N20" s="14"/>
       <c r="O20" s="10"/>
-      <c r="P20" s="34"/>
-      <c r="Q20" s="10"/>
+      <c r="P20" s="10"/>
+      <c r="Q20" s="34"/>
       <c r="R20" s="10"/>
       <c r="S20" s="10"/>
       <c r="T20" s="10"/>
-      <c r="U20" s="14"/>
-      <c r="V20" s="10"/>
+      <c r="U20" s="10"/>
+      <c r="V20" s="14"/>
       <c r="W20" s="10"/>
       <c r="X20" s="10"/>
-      <c r="Y20" s="20"/>
-    </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y20" s="10"/>
+      <c r="Z20" s="20"/>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
       <c r="B21" s="9"/>
       <c r="C21" s="22"/>
       <c r="D21" s="22"/>
       <c r="E21" s="22"/>
       <c r="F21" s="22"/>
-      <c r="G21" s="8"/>
+      <c r="G21" s="22"/>
       <c r="H21" s="8"/>
       <c r="I21" s="8"/>
       <c r="J21" s="8"/>
       <c r="K21" s="8"/>
       <c r="L21" s="8"/>
-      <c r="M21" s="14"/>
-      <c r="N21" s="10"/>
+      <c r="M21" s="8"/>
+      <c r="N21" s="14"/>
       <c r="O21" s="10"/>
-      <c r="P21" s="34"/>
-      <c r="Q21" s="10"/>
+      <c r="P21" s="10"/>
+      <c r="Q21" s="34"/>
       <c r="R21" s="10"/>
       <c r="S21" s="10"/>
       <c r="T21" s="10"/>
-      <c r="U21" s="14"/>
-      <c r="V21" s="10"/>
+      <c r="U21" s="10"/>
+      <c r="V21" s="14"/>
       <c r="W21" s="10"/>
       <c r="X21" s="10"/>
-      <c r="Y21" s="20"/>
-    </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y21" s="10"/>
+      <c r="Z21" s="20"/>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
       <c r="B22" s="9"/>
       <c r="C22" s="22"/>
       <c r="D22" s="22"/>
       <c r="E22" s="22"/>
       <c r="F22" s="22"/>
-      <c r="G22" s="8"/>
+      <c r="G22" s="22"/>
       <c r="H22" s="8"/>
       <c r="I22" s="8"/>
       <c r="J22" s="8"/>
       <c r="K22" s="8"/>
       <c r="L22" s="8"/>
-      <c r="M22" s="14"/>
-      <c r="N22" s="10"/>
+      <c r="M22" s="8"/>
+      <c r="N22" s="14"/>
       <c r="O22" s="10"/>
-      <c r="P22" s="34"/>
-      <c r="Q22" s="10"/>
+      <c r="P22" s="10"/>
+      <c r="Q22" s="34"/>
       <c r="R22" s="10"/>
       <c r="S22" s="10"/>
       <c r="T22" s="10"/>
-      <c r="U22" s="14"/>
-      <c r="V22" s="10"/>
+      <c r="U22" s="10"/>
+      <c r="V22" s="14"/>
       <c r="W22" s="10"/>
       <c r="X22" s="10"/>
-      <c r="Y22" s="20"/>
-    </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y22" s="10"/>
+      <c r="Z22" s="20"/>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
       <c r="B23" s="9"/>
       <c r="C23" s="22"/>
       <c r="D23" s="22"/>
       <c r="E23" s="22"/>
       <c r="F23" s="22"/>
-      <c r="G23" s="8"/>
+      <c r="G23" s="22"/>
       <c r="H23" s="8"/>
       <c r="I23" s="8"/>
       <c r="J23" s="8"/>
       <c r="K23" s="8"/>
       <c r="L23" s="8"/>
-      <c r="M23" s="14"/>
-      <c r="N23" s="10"/>
+      <c r="M23" s="8"/>
+      <c r="N23" s="14"/>
       <c r="O23" s="10"/>
-      <c r="P23" s="34"/>
-      <c r="Q23" s="10"/>
+      <c r="P23" s="10"/>
+      <c r="Q23" s="34"/>
       <c r="R23" s="10"/>
       <c r="S23" s="10"/>
       <c r="T23" s="10"/>
-      <c r="U23" s="14"/>
-      <c r="V23" s="10"/>
+      <c r="U23" s="10"/>
+      <c r="V23" s="14"/>
       <c r="W23" s="10"/>
       <c r="X23" s="10"/>
-      <c r="Y23" s="20"/>
-    </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y23" s="10"/>
+      <c r="Z23" s="20"/>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
       <c r="B24" s="9"/>
       <c r="C24" s="22"/>
       <c r="D24" s="22"/>
       <c r="E24" s="22"/>
       <c r="F24" s="22"/>
-      <c r="G24" s="8"/>
+      <c r="G24" s="22"/>
       <c r="H24" s="8"/>
       <c r="I24" s="8"/>
       <c r="J24" s="8"/>
       <c r="K24" s="8"/>
       <c r="L24" s="8"/>
-      <c r="M24" s="14"/>
-      <c r="N24" s="10"/>
+      <c r="M24" s="8"/>
+      <c r="N24" s="14"/>
       <c r="O24" s="10"/>
-      <c r="P24" s="34"/>
-      <c r="Q24" s="10"/>
+      <c r="P24" s="10"/>
+      <c r="Q24" s="34"/>
       <c r="R24" s="10"/>
       <c r="S24" s="10"/>
       <c r="T24" s="10"/>
-      <c r="U24" s="14"/>
-      <c r="V24" s="10"/>
+      <c r="U24" s="10"/>
+      <c r="V24" s="14"/>
       <c r="W24" s="10"/>
       <c r="X24" s="10"/>
-      <c r="Y24" s="20"/>
-    </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y24" s="10"/>
+      <c r="Z24" s="20"/>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25" s="8"/>
       <c r="B25" s="9"/>
       <c r="C25" s="22"/>
       <c r="D25" s="22"/>
       <c r="E25" s="22"/>
       <c r="F25" s="22"/>
-      <c r="G25" s="8"/>
+      <c r="G25" s="22"/>
       <c r="H25" s="8"/>
       <c r="I25" s="8"/>
       <c r="J25" s="8"/>
       <c r="K25" s="8"/>
       <c r="L25" s="8"/>
-      <c r="M25" s="14"/>
-      <c r="N25" s="10"/>
+      <c r="M25" s="8"/>
+      <c r="N25" s="14"/>
       <c r="O25" s="10"/>
-      <c r="P25" s="34"/>
-      <c r="Q25" s="10"/>
+      <c r="P25" s="10"/>
+      <c r="Q25" s="34"/>
       <c r="R25" s="10"/>
       <c r="S25" s="10"/>
       <c r="T25" s="10"/>
-      <c r="U25" s="14"/>
-      <c r="V25" s="10"/>
+      <c r="U25" s="10"/>
+      <c r="V25" s="14"/>
       <c r="W25" s="10"/>
       <c r="X25" s="10"/>
-      <c r="Y25" s="20"/>
-    </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y25" s="10"/>
+      <c r="Z25" s="20"/>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
       <c r="B26" s="9"/>
       <c r="C26" s="22"/>
       <c r="D26" s="22"/>
       <c r="E26" s="22"/>
       <c r="F26" s="22"/>
-      <c r="G26" s="8"/>
+      <c r="G26" s="22"/>
       <c r="H26" s="8"/>
       <c r="I26" s="8"/>
       <c r="J26" s="8"/>
       <c r="K26" s="8"/>
       <c r="L26" s="8"/>
-      <c r="M26" s="14"/>
-      <c r="N26" s="10"/>
+      <c r="M26" s="8"/>
+      <c r="N26" s="14"/>
       <c r="O26" s="10"/>
-      <c r="P26" s="34"/>
-      <c r="Q26" s="10"/>
+      <c r="P26" s="10"/>
+      <c r="Q26" s="34"/>
       <c r="R26" s="10"/>
       <c r="S26" s="10"/>
       <c r="T26" s="10"/>
-      <c r="U26" s="14"/>
-      <c r="V26" s="10"/>
+      <c r="U26" s="10"/>
+      <c r="V26" s="14"/>
       <c r="W26" s="10"/>
       <c r="X26" s="10"/>
-      <c r="Y26" s="20"/>
-    </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y26" s="10"/>
+      <c r="Z26" s="20"/>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A27" s="8"/>
       <c r="B27" s="9"/>
       <c r="C27" s="22"/>
       <c r="D27" s="22"/>
       <c r="E27" s="22"/>
       <c r="F27" s="22"/>
-      <c r="G27" s="8"/>
+      <c r="G27" s="22"/>
       <c r="H27" s="8"/>
       <c r="I27" s="8"/>
       <c r="J27" s="8"/>
       <c r="K27" s="8"/>
       <c r="L27" s="8"/>
-      <c r="M27" s="14"/>
-      <c r="N27" s="10"/>
+      <c r="M27" s="8"/>
+      <c r="N27" s="14"/>
       <c r="O27" s="10"/>
-      <c r="P27" s="34"/>
-      <c r="Q27" s="10"/>
+      <c r="P27" s="10"/>
+      <c r="Q27" s="34"/>
       <c r="R27" s="10"/>
       <c r="S27" s="10"/>
       <c r="T27" s="10"/>
-      <c r="U27" s="14"/>
-      <c r="V27" s="10"/>
+      <c r="U27" s="10"/>
+      <c r="V27" s="14"/>
       <c r="W27" s="10"/>
       <c r="X27" s="10"/>
-      <c r="Y27" s="20"/>
-    </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y27" s="10"/>
+      <c r="Z27" s="20"/>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A28" s="8"/>
       <c r="B28" s="9"/>
       <c r="C28" s="22"/>
       <c r="D28" s="22"/>
       <c r="E28" s="22"/>
       <c r="F28" s="22"/>
-      <c r="G28" s="8"/>
+      <c r="G28" s="22"/>
       <c r="H28" s="8"/>
       <c r="I28" s="8"/>
       <c r="J28" s="8"/>
       <c r="K28" s="8"/>
       <c r="L28" s="8"/>
-      <c r="M28" s="14"/>
-      <c r="N28" s="10"/>
+      <c r="M28" s="8"/>
+      <c r="N28" s="14"/>
       <c r="O28" s="10"/>
-      <c r="P28" s="34"/>
-      <c r="Q28" s="10"/>
+      <c r="P28" s="10"/>
+      <c r="Q28" s="34"/>
       <c r="R28" s="10"/>
       <c r="S28" s="10"/>
       <c r="T28" s="10"/>
-      <c r="U28" s="14"/>
-      <c r="V28" s="10"/>
+      <c r="U28" s="10"/>
+      <c r="V28" s="14"/>
       <c r="W28" s="10"/>
       <c r="X28" s="10"/>
-      <c r="Y28" s="20"/>
-    </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y28" s="10"/>
+      <c r="Z28" s="20"/>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A29" s="8"/>
       <c r="B29" s="9"/>
       <c r="C29" s="22"/>
       <c r="D29" s="22"/>
       <c r="E29" s="22"/>
       <c r="F29" s="22"/>
-      <c r="G29" s="8"/>
+      <c r="G29" s="22"/>
       <c r="H29" s="8"/>
       <c r="I29" s="8"/>
       <c r="J29" s="8"/>
       <c r="K29" s="8"/>
       <c r="L29" s="8"/>
-      <c r="M29" s="14"/>
-      <c r="N29" s="10"/>
+      <c r="M29" s="8"/>
+      <c r="N29" s="14"/>
       <c r="O29" s="10"/>
-      <c r="P29" s="34"/>
-      <c r="Q29" s="10"/>
+      <c r="P29" s="10"/>
+      <c r="Q29" s="34"/>
       <c r="R29" s="10"/>
       <c r="S29" s="10"/>
       <c r="T29" s="10"/>
-      <c r="U29" s="14"/>
-      <c r="V29" s="10"/>
+      <c r="U29" s="10"/>
+      <c r="V29" s="14"/>
       <c r="W29" s="10"/>
       <c r="X29" s="10"/>
-      <c r="Y29" s="20"/>
-    </row>
-    <row r="30" spans="1:25" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="46" t="s">
+      <c r="Y29" s="10"/>
+      <c r="Z29" s="20"/>
+    </row>
+    <row r="30" spans="1:26" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B30" s="47"/>
-      <c r="C30" s="47"/>
-      <c r="D30" s="47"/>
-      <c r="E30" s="47"/>
-      <c r="F30" s="47"/>
-      <c r="G30" s="47"/>
-      <c r="H30" s="47"/>
-      <c r="I30" s="47"/>
-      <c r="J30" s="47"/>
-      <c r="K30" s="47"/>
-      <c r="L30" s="48"/>
-      <c r="M30" s="15">
-        <f>SUM(M$6:M29)</f>
-        <v>0</v>
-      </c>
-      <c r="N30" s="16">
+      <c r="B30" s="39"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="39"/>
+      <c r="E30" s="39"/>
+      <c r="F30" s="39"/>
+      <c r="G30" s="39"/>
+      <c r="H30" s="39"/>
+      <c r="I30" s="39"/>
+      <c r="J30" s="39"/>
+      <c r="K30" s="39"/>
+      <c r="L30" s="39"/>
+      <c r="M30" s="40"/>
+      <c r="N30" s="15">
         <f>SUM(N$6:N29)</f>
         <v>0</v>
       </c>
-      <c r="O30" s="16"/>
-      <c r="P30" s="35"/>
-      <c r="Q30" s="16"/>
-      <c r="R30" s="11">
-        <f>SUM(R$6:R29)</f>
+      <c r="O30" s="16">
+        <f>SUM(O$6:O29)</f>
         <v>0</v>
       </c>
-      <c r="S30" s="27"/>
-      <c r="T30" s="27">
-        <f xml:space="preserve"> SUM(T$6:T29)</f>
+      <c r="P30" s="16"/>
+      <c r="Q30" s="35"/>
+      <c r="R30" s="16"/>
+      <c r="S30" s="11">
+        <f>SUM(S$6:S29)</f>
         <v>0</v>
       </c>
-      <c r="U30" s="15"/>
-      <c r="V30" s="11">
-        <f>SUM(V$6:V29)</f>
+      <c r="T30" s="27"/>
+      <c r="U30" s="27">
+        <f xml:space="preserve"> SUM(U$6:U29)</f>
         <v>0</v>
       </c>
-      <c r="W30" s="11"/>
-      <c r="X30" s="11">
-        <f>SUM(X$6:X29)</f>
+      <c r="V30" s="15"/>
+      <c r="W30" s="11">
+        <f>SUM(W$6:W29)</f>
         <v>0</v>
       </c>
+      <c r="X30" s="11"/>
       <c r="Y30" s="11">
-        <f>SUM($Y$6:Y29)</f>
+        <f>SUM(Y$6:Y29)</f>
         <v>0</v>
       </c>
+      <c r="Z30" s="11">
+        <f>SUM($Z$6:Z29)</f>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="23">
-    <mergeCell ref="A1:V1"/>
-    <mergeCell ref="A30:L30"/>
+  <mergeCells count="24">
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="Z4:Z5"/>
+    <mergeCell ref="M4:M5"/>
+    <mergeCell ref="R4:S4"/>
+    <mergeCell ref="V4:W4"/>
+    <mergeCell ref="X4:Y4"/>
+    <mergeCell ref="Q4:Q5"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="A1:W1"/>
+    <mergeCell ref="A30:M30"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="F4:F5"/>
     <mergeCell ref="H4:H5"/>
     <mergeCell ref="I4:I5"/>
     <mergeCell ref="J4:J5"/>
     <mergeCell ref="K4:K5"/>
-    <mergeCell ref="S4:T4"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="M4:M5"/>
+    <mergeCell ref="L4:L5"/>
+    <mergeCell ref="T4:U4"/>
+    <mergeCell ref="G4:G5"/>
     <mergeCell ref="N4:N5"/>
-    <mergeCell ref="Y4:Y5"/>
-    <mergeCell ref="L4:L5"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="U4:V4"/>
-    <mergeCell ref="W4:X4"/>
-    <mergeCell ref="P4:P5"/>
     <mergeCell ref="O4:O5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>